<commit_message>
Fixe a HotGo-Validando Errores
</commit_message>
<xml_diff>
--- a/src/assets/files/payment_commit_missing_modelo.xlsx
+++ b/src/assets/files/payment_commit_missing_modelo.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Sites\clx-portalv2\src\assets\files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gtanoira\eclipse-workspace\CLX-Documentacion\app-HotGoDatawarehouse\Documentacion\TablasModelo_Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="35">
   <si>
     <t>userId</t>
   </si>
@@ -108,9 +108,6 @@
   </si>
   <si>
     <t>ccm</t>
-  </si>
-  <si>
-    <t>auto</t>
   </si>
   <si>
     <t>payment_commit</t>
@@ -149,6 +146,12 @@
       </rPr>
       <t xml:space="preserve"> son opcionales, el resto es obligatorio (no pueden estar vacías)</t>
     </r>
+  </si>
+  <si>
+    <t>isSuscription</t>
+  </si>
+  <si>
+    <t>online</t>
   </si>
 </sst>
 </file>
@@ -560,11 +563,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q9"/>
+  <dimension ref="A1:R9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B9" sqref="B9"/>
+      <selection pane="bottomLeft" activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -582,9 +585,10 @@
     <col min="11" max="11" width="21.88671875" style="8" customWidth="1"/>
     <col min="12" max="12" width="20.33203125" customWidth="1"/>
     <col min="14" max="14" width="36.21875" customWidth="1"/>
+    <col min="18" max="18" width="17" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -636,10 +640,13 @@
       <c r="Q1" s="10" t="s">
         <v>23</v>
       </c>
+      <c r="R1" s="3" t="s">
+        <v>33</v>
+      </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>25</v>
@@ -657,14 +664,14 @@
         <v>150</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="H2" s="2">
         <v>30</v>
       </c>
       <c r="I2" s="4"/>
       <c r="J2" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="K2" s="8">
         <v>43322.634722222225</v>
@@ -673,13 +680,16 @@
         <v>0</v>
       </c>
       <c r="N2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="P2">
         <v>0</v>
       </c>
+      <c r="R2" s="2">
+        <v>1</v>
+      </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A4" s="6" t="s">
         <v>5</v>
       </c>
@@ -687,7 +697,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A5" s="6" t="s">
         <v>6</v>
       </c>
@@ -695,7 +705,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A6" s="6" t="s">
         <v>7</v>
       </c>
@@ -703,7 +713,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A7" s="6" t="s">
         <v>9</v>
       </c>
@@ -711,15 +721,15 @@
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A8" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="B8" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="B8" s="11" t="s">
-        <v>33</v>
-      </c>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:18" x14ac:dyDescent="0.3">
       <c r="B9" s="13"/>
     </row>
   </sheetData>

</xml_diff>